<commit_message>
Did some call changes
</commit_message>
<xml_diff>
--- a/reports/error_report.xlsx
+++ b/reports/error_report.xlsx
@@ -319,28 +319,28 @@
     <t>LLM-enhanced review of spelling/grammar:</t>
   </si>
   <si>
-    <t>Variants found: {'Title Insurance', 'Title Ins', 'Title Association'}</t>
-  </si>
-  <si>
-    <t>Variants found: {'This Privacy', 'This Notice', 'This Commitment', 'This\nCommitment'}</t>
-  </si>
-  <si>
-    <t>Variants found: {'Commitment Conditions', 'Commitment\nCondition', 'Commitment Date', 'Commitment Condition'}</t>
-  </si>
-  <si>
-    <t>Variants found: {'Proposed Policy', 'Proposed Amount', 'Proposed Insured'}</t>
-  </si>
-  <si>
-    <t>Variants found: {'President\nAuthorized', 'President\nAttest'}</t>
+    <t>Variants found: {'Title Association', 'Title Ins', 'Title Insurance'}</t>
+  </si>
+  <si>
+    <t>Variants found: {'This\nCommitment', 'This Privacy', 'This Notice', 'This Commitment'}</t>
+  </si>
+  <si>
+    <t>Variants found: {'Commitment\nCondition', 'Commitment Conditions', 'Commitment Condition', 'Commitment Date'}</t>
+  </si>
+  <si>
+    <t>Variants found: {'Proposed Insured', 'Proposed Amount', 'Proposed Policy'}</t>
+  </si>
+  <si>
+    <t>Variants found: {'President\nAttest', 'President\nAuthorized'}</t>
   </si>
   <si>
     <t>Variants found: {'Main Phone', 'Main Fax'}</t>
   </si>
   <si>
-    <t>Variants found: {'The Land', 'The Proposed', 'The West', 'The State', 'The Title', 'The Company', 'The Policy', 'The Service', 'The\nPrivacy'}</t>
-  </si>
-  <si>
-    <t>Variants found: {'Real Property', 'Real Estate'}</t>
+    <t>Variants found: {'The Policy', 'The West', 'The\nPrivacy', 'The Company', 'The Service', 'The Proposed', 'The Title', 'The State', 'The Land'}</t>
+  </si>
+  <si>
+    <t>Variants found: {'Real Estate', 'Real Property'}</t>
   </si>
   <si>
     <t>Variants found: {'Special Exceptions', 'Special Coverage'}</t>
@@ -352,19 +352,19 @@
     <t>Variants found: {'Caryl Halfwassen', 'Caryl\nHalfwassen'}</t>
   </si>
   <si>
-    <t>Variants found: {'Internet Protocol', 'Internet Crime'}</t>
-  </si>
-  <si>
-    <t>Variants found: {'Privacy Statement', 'Privacy Notice', 'Privacy Inquiry', 'Privacy\nNotice'}</t>
-  </si>
-  <si>
-    <t>Variants found: {'Personal\nInformation', 'Personal Information'}</t>
+    <t>Variants found: {'Internet Crime', 'Internet Protocol'}</t>
+  </si>
+  <si>
+    <t>Variants found: {'Privacy\nNotice', 'Privacy Statement', 'Privacy Notice', 'Privacy Inquiry'}</t>
+  </si>
+  <si>
+    <t>Variants found: {'Personal Information', 'Personal\nInformation'}</t>
   </si>
   <si>
     <t>Variants found: {'Browsing\nInformation', 'Browsing Information'}</t>
   </si>
   <si>
-    <t>Variants found: {'Other Online', 'Other Sites', 'Other Counties'}</t>
+    <t>Variants found: {'Other Counties', 'Other Sites', 'Other Online'}</t>
   </si>
   <si>
     <t>Variants found: {'Do Not', 'Do\nNot'}</t>
@@ -373,7 +373,7 @@
     <t>Variants found: {'Your Consent', 'Your Information'}</t>
   </si>
   <si>
-    <t>Variants found: {'For California', 'For Virginia', 'For Nevada', 'For Oregon'}</t>
+    <t>Variants found: {'For Virginia', 'For Nevada', 'For Oregon', 'For California'}</t>
   </si>
   <si>
     <t>Variants found: {'Nebraska Form', 'Nebraska\nCourtesy'}</t>
@@ -550,12 +550,7 @@
     <t>How nor, Own or, Town or, Down or, How or, Shown or, Horn or, Gown or, Hewn or, Sown or, Howl or, Mown or, Hows or, HON or, Hoon or, Howe or, Hon or</t>
   </si>
   <si>
-    <t xml:space="preserve">LLM enhancement unavailable. Error: 
-You tried to access openai.ChatCompletion, but this is no longer supported in openai&gt;=1.0.0 - see the README at https://github.com/openai/openai-python for the API.
-You can run `openai migrate` to automatically upgrade your codebase to use the 1.0.0 interface. 
-Alternatively, you can pin your installation to the old version, e.g. `pip install openai==0.28`
-A detailed migration guide is available here: https://github.com/openai/openai-python/discussions/742
-</t>
+    <t>LLM enhancement unavailable. Error: Error code: 429 - {'error': {'message': 'You exceeded your current quota, please check your plan and billing details. For more information on this error, read the docs: https://platform.openai.com/docs/guides/error-codes/api-errors.', 'type': 'insufficient_quota', 'param': None, 'code': 'insufficient_quota'}}</t>
   </si>
   <si>
     <t>Could not resolve name variation via LLM.</t>
@@ -567,12 +562,7 @@
     <t>Please add this information</t>
   </si>
   <si>
-    <t xml:space="preserve">LLM error: 
-You tried to access openai.ChatCompletion, but this is no longer supported in openai&gt;=1.0.0 - see the README at https://github.com/openai/openai-python for the API.
-You can run `openai migrate` to automatically upgrade your codebase to use the 1.0.0 interface. 
-Alternatively, you can pin your installation to the old version, e.g. `pip install openai==0.28`
-A detailed migration guide is available here: https://github.com/openai/openai-python/discussions/742
-</t>
+    <t>LLM error: Error code: 429 - {'error': {'message': 'You exceeded your current quota, please check your plan and billing details. For more information on this error, read the docs: https://platform.openai.com/docs/guides/error-codes/api-errors.', 'type': 'insufficient_quota', 'param': None, 'code': 'insufficient_quota'}}</t>
   </si>
 </sst>
 </file>

</xml_diff>